<commit_message>
2020 Media Finished, Final Script in Flow
</commit_message>
<xml_diff>
--- a/input/Input_072020.xlsx
+++ b/input/Input_072020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/east_alexander_epa_gov/Documents/Profile/Desktop/LEM4/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aeast\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\LEM4\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{AEB5DC28-DBF4-4CEF-94C6-B4ED01FC88B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{DB4A8FCB-62C3-46A4-B172-3999099E9939}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{AEB5DC28-DBF4-4CEF-94C6-B4ED01FC88B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E6542CD0-5F83-4A1C-8462-D72966BC519C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{954D9476-CD18-4396-BAEA-D273523A90CB}"/>
   </bookViews>
@@ -1957,7 +1957,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2044,7 +2044,7 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>20000</v>
       </c>
       <c r="C2">
         <v>0.1</v>
@@ -2104,7 +2104,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>20000</v>
       </c>
       <c r="C3">
         <v>0.05</v>
@@ -2164,7 +2164,7 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>20000</v>
       </c>
       <c r="C4">
         <v>0.05</v>
@@ -23397,6 +23397,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Records_x0020_Date xmlns="e6ae508a-59c9-42bb-b4fe-819888132927" xsi:nil="true"/>
+    <Records_x0020_Status xmlns="e6ae508a-59c9-42bb-b4fe-819888132927">Pending</Records_x0020_Status>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100175F8EE2D16CCF4E9795DBA2E0366580" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0e36aa337ceae7f1d93f3efc48c3ea9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e6ae508a-59c9-42bb-b4fe-819888132927" xmlns:ns4="7d98c609-804a-400c-9f9b-45f6e3b4e0b0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="376aea29d8ef60d7b2126687d24b7c91" ns3:_="" ns4:_="">
     <xsd:import namespace="e6ae508a-59c9-42bb-b4fe-819888132927"/>
@@ -23605,15 +23614,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Records_x0020_Date xmlns="e6ae508a-59c9-42bb-b4fe-819888132927" xsi:nil="true"/>
-    <Records_x0020_Status xmlns="e6ae508a-59c9-42bb-b4fe-819888132927">Pending</Records_x0020_Status>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -23624,6 +23624,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619936EC-EF42-4CC2-B464-377D7CE891A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e6ae508a-59c9-42bb-b4fe-819888132927"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7d98c609-804a-400c-9f9b-45f6e3b4e0b0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ECAB6FE-ED10-48D6-B2FD-BD0018793311}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23642,23 +23659,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619936EC-EF42-4CC2-B464-377D7CE891A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7d98c609-804a-400c-9f9b-45f6e3b4e0b0"/>
-    <ds:schemaRef ds:uri="e6ae508a-59c9-42bb-b4fe-819888132927"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A602FC1-DACC-4B1D-A27E-1705833C36F6}">
   <ds:schemaRefs>

</xml_diff>